<commit_message>
ajuste de meta con licencia especial
</commit_message>
<xml_diff>
--- a/data/export/nominas.xlsx
+++ b/data/export/nominas.xlsx
@@ -585,12 +585,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>prueba 100</t>
+          <t>LIcencia rre especial aprobada por el directorio</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>101</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -604,16 +604,16 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="R2" t="n">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="S2" t="n">
-        <v>3900000</v>
+        <v>3300000</v>
       </c>
       <c r="T2" t="n">
-        <v>3900000</v>
+        <v>3300000</v>
       </c>
       <c r="U2" t="inlineStr"/>
     </row>
@@ -662,8 +662,16 @@
       <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>LIcencia rre especial aprobada por el directorio</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr">
         <is>
           <t>No</t>
@@ -675,16 +683,16 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="R3" t="n">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="S3" t="n">
-        <v>27500000</v>
+        <v>24750000</v>
       </c>
       <c r="T3" t="n">
-        <v>27500000</v>
+        <v>24750000</v>
       </c>
       <c r="U3" t="inlineStr"/>
     </row>
@@ -12366,12 +12374,12 @@
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>prueba 100</t>
+          <t>LIcencia rre especial aprobada por el directorio</t>
         </is>
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>101</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -12385,16 +12393,16 @@
         </is>
       </c>
       <c r="Q165" t="n">
-        <v>18</v>
+        <v>15.5</v>
       </c>
       <c r="R165" t="n">
-        <v>18</v>
+        <v>15.5</v>
       </c>
       <c r="S165" t="n">
-        <v>19112500</v>
+        <v>16245625</v>
       </c>
       <c r="T165" t="n">
-        <v>19112500</v>
+        <v>16245625</v>
       </c>
       <c r="U165" t="inlineStr"/>
     </row>

</xml_diff>